<commit_message>
Chart reading test workbooks
git-svn-id: https://phpexcel.svn.codeplex.com/svn/trunk@86720 2327b42d-5241-43d6-9e2a-de5ac946f064
</commit_message>
<xml_diff>
--- a/Tests/templates/32chartreadwrite.xlsx
+++ b/Tests/templates/32chartreadwrite.xlsx
@@ -259,9 +259,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.4544534875009653E-2"/>
+          <c:x val="7.4620653261187692E-2"/>
           <c:y val="0.14738996929375636"/>
-          <c:w val="0.78950293943705463"/>
+          <c:w val="0.79942686120554851"/>
           <c:h val="0.68817369909979531"/>
         </c:manualLayout>
       </c:layout>
@@ -369,40 +369,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1500</c:v>
+                  <c:v>1690</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1700</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>1570</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2490</c:v>
+                  <c:v>3270</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>610</c:v>
+                  <c:v>2860</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>1910</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3130</c:v>
+                  <c:v>3120</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3380</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3000</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1360</c:v>
+                  <c:v>1920</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3100</c:v>
+                  <c:v>950</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2400</c:v>
+                  <c:v>2360</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -510,40 +510,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2640</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>740</c:v>
+                  <c:v>3480</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1060</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2160</c:v>
+                  <c:v>2360</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2130</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1340</c:v>
+                  <c:v>2080</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>720</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1130</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1900</c:v>
+                  <c:v>2790</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2970</c:v>
+                  <c:v>3230</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1130</c:v>
+                  <c:v>1790</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>940</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -651,40 +651,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1510</c:v>
+                  <c:v>3040</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2110</c:v>
+                  <c:v>2180</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2560</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3380</c:v>
+                  <c:v>3390</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1160</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2570</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1810</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1890</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2250</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1210</c:v>
+                  <c:v>1460</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1060</c:v>
+                  <c:v>1820</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3230</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,40 +733,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>770</c:v>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2210</c:v>
+                  <c:v>1730</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2160</c:v>
+                  <c:v>2770</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2340</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1450</c:v>
+                  <c:v>950</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2520</c:v>
+                  <c:v>2070</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1320</c:v>
+                  <c:v>1260</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>900</c:v>
+                  <c:v>3140</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3500</c:v>
+                  <c:v>680</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>1090</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>2250</c:v>
+                  <c:v>1330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -783,11 +783,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88728704"/>
-        <c:axId val="88731008"/>
+        <c:axId val="80094336"/>
+        <c:axId val="80096640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88728704"/>
+        <c:axId val="80094336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,7 +836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88731008"/>
+        <c:crossAx val="80096640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -844,7 +844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88731008"/>
+        <c:axId val="80096640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,7 +894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88728704"/>
+        <c:crossAx val="80094336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -908,7 +908,7 @@
           <c:x val="0.88880180056427871"/>
           <c:y val="0.43398164061979561"/>
           <c:w val="9.8125848033438337E-2"/>
-          <c:h val="9.8259979529170982E-2"/>
+          <c:h val="0.15002397279007881"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -944,10 +944,10 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -966,6 +966,94 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>549044</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="182880"/>
+          <a:ext cx="1158644" cy="1249680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53340" y="4960620"/>
+          <a:ext cx="2659380" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1351,51 +1439,51 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:M7" ca="1" si="0">(RANDBETWEEN(-50,250)+100)*10</f>
-        <v>1500</v>
+        <v>1690</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>1700</v>
+        <v>2100</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>2000</v>
+        <v>1570</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>2490</v>
+        <v>3270</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>610</v>
+        <v>2860</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>600</v>
+        <v>1910</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>3130</v>
+        <v>3120</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>3380</v>
+        <v>660</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>3000</v>
+        <v>1080</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>1360</v>
+        <v>1920</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>3100</v>
+        <v>950</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>2400</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1404,51 +1492,51 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>2640</v>
+        <v>1310</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>740</v>
+        <v>3480</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>1060</v>
+        <v>510</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>2160</v>
+        <v>2360</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>2130</v>
+        <v>2200</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>1340</v>
+        <v>2080</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>720</v>
+        <v>2100</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>1130</v>
+        <v>2700</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>1900</v>
+        <v>2790</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>2970</v>
+        <v>3230</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>1130</v>
+        <v>1790</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>940</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1457,51 +1545,51 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>1510</v>
+        <v>3040</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>2110</v>
+        <v>2180</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2560</v>
+        <v>2300</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>3380</v>
+        <v>3390</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1160</v>
+        <v>570</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
+        <v>2570</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
         <v>1810</v>
       </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1890</v>
-      </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>800</v>
+        <v>520</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>2250</v>
+        <v>660</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>1210</v>
+        <v>1460</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>1060</v>
+        <v>1820</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
-        <v>3230</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1510,51 +1598,51 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>770</v>
+        <v>1440</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2210</v>
+        <v>1730</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>2160</v>
+        <v>2770</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>2340</v>
+        <v>510</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>1450</v>
+        <v>950</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>2520</v>
+        <v>2070</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>1320</v>
+        <v>1260</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>900</v>
+        <v>3140</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>3500</v>
+        <v>680</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
+        <v>860</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="0"/>
         <v>800</v>
       </c>
-      <c r="L7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1090</v>
-      </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>2250</v>
+        <v>1330</v>
       </c>
     </row>
   </sheetData>
@@ -1574,9 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG32" sqref="AG32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>